<commit_message>
Auto-committed on 2023/03/13 週一 11:50:34.99
</commit_message>
<xml_diff>
--- a/Program/Other/LM030_底稿_轉催收案件明細_核定總表.xlsx
+++ b/Program/Other/LM030_底稿_轉催收案件明細_核定總表.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2896C984-22B4-4F12-940E-9A04D45006F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
   </bookViews>
   <sheets>
-    <sheet name="11005" sheetId="1" r:id="rId1"/>
+    <sheet name="YYYMM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'11005'!$A$2:$N$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">YYYMM!$A$2:$N$4</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'11005'!$A$1:$M$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">YYYMM!$A$1:$M$10</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -95,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -404,11 +403,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般 2" xfId="2"/>
     <cellStyle name="千分位" xfId="1" builtinId="3"/>
-    <cellStyle name="千分位 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="千分位 2" xfId="3"/>
     <cellStyle name="百分比" xfId="5" builtinId="5"/>
-    <cellStyle name="貨幣 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="貨幣 2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -499,23 +498,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -551,23 +533,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -743,7 +708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -754,23 +719,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="27" customWidth="1"/>
+    <col min="1" max="1" width="8.6328125" style="27" customWidth="1"/>
     <col min="2" max="2" width="11" style="27" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="24" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
-    <col min="10" max="11" width="9.6640625" style="24" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="27" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="5.36328125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" style="24" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" style="26" customWidth="1"/>
+    <col min="10" max="11" width="9.6328125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="9.6328125" style="27" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="3" customFormat="1" ht="27.5" x14ac:dyDescent="0.4">
       <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
@@ -804,7 +769,7 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -861,7 +826,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -876,7 +841,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="31"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
@@ -890,7 +855,7 @@
       <c r="L4" s="19"/>
       <c r="M4" s="21"/>
     </row>
-    <row r="11" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="27"/>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
@@ -906,7 +871,7 @@
       <c r="M11"/>
       <c r="N11" s="22"/>
     </row>
-    <row r="12" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="27"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -922,7 +887,7 @@
       <c r="M12"/>
       <c r="N12" s="22"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.4">
       <c r="N13" s="28"/>
       <c r="O13" s="27"/>
       <c r="P13" s="27"/>
@@ -931,7 +896,7 @@
       <c r="S13" s="27"/>
       <c r="T13" s="27"/>
     </row>
-    <row r="14" spans="1:30" s="33" customFormat="1" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="33" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A14" s="27"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -947,7 +912,7 @@
       <c r="M14"/>
       <c r="N14" s="32"/>
     </row>
-    <row r="15" spans="1:30" s="33" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="33" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="27"/>
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
@@ -963,7 +928,7 @@
       <c r="M15"/>
       <c r="N15" s="32"/>
     </row>
-    <row r="16" spans="1:30" s="34" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="34" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="27"/>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -978,7 +943,7 @@
       <c r="L16" s="27"/>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="27"/>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
@@ -994,7 +959,7 @@
       <c r="M17"/>
       <c r="N17" s="29"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
       <c r="N18" s="28"/>
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
@@ -1003,7 +968,7 @@
       <c r="S18" s="27"/>
       <c r="T18" s="27"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
       <c r="N19" s="28"/>
       <c r="O19" s="27"/>
       <c r="P19" s="27"/>
@@ -1013,7 +978,7 @@
       <c r="T19" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:N4"/>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
   </mergeCells>

</xml_diff>